<commit_message>
Added Phone Numbers to Insurance Company; Added PaRequestNotes and PaRequestNotes_Audit
</commit_message>
<xml_diff>
--- a/LMS_PAManage/site/src/assets/pa_request_template.xlsx
+++ b/LMS_PAManage/site/src/assets/pa_request_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\LIMSManagement\LMS_PAManage\site\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\LMSManagement\LMS_PAManage\site\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6B85E706-25C8-4FE2-8837-2AEAB8E66B6E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180E4035-987D-4DF2-8ACD-074F2081BC5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6255" yWindow="8505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,16 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>TP</t>
-  </si>
-  <si>
     <t>PATIENT</t>
   </si>
   <si>
     <t>DRUG NAME</t>
   </si>
   <si>
-    <t>NOTES</t>
+    <t>INSURACE CODE</t>
+  </si>
+  <si>
+    <t>PHYSICIAN</t>
   </si>
 </sst>
 </file>
@@ -424,12 +424,13 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
@@ -442,16 +443,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -1689,9 +1690,7 @@
       <c r="I113" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G1:I1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Pa Notes and Claim Upload functionality
</commit_message>
<xml_diff>
--- a/LMS_PAManage/site/src/assets/pa_request_template.xlsx
+++ b/LMS_PAManage/site/src/assets/pa_request_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\LMSManagement\LMS_PAManage\site\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180E4035-987D-4DF2-8ACD-074F2081BC5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A40C7B2-6D34-492A-8442-663056932A3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="8505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
     <t>DRUG NAME</t>
   </si>
   <si>
-    <t>INSURACE CODE</t>
+    <t>PHYSICIAN</t>
   </si>
   <si>
-    <t>PHYSICIAN</t>
+    <t>INSURANCE CODE</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +443,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>

</xml_diff>